<commit_message>
added basic data display and run info into frame title
</commit_message>
<xml_diff>
--- a/CATE Template - Multi Run.xlsx
+++ b/CATE Template - Multi Run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" calcOnSave="0"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -53,7 +53,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,16 +74,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -138,13 +149,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -153,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -170,11 +196,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -483,7 +514,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,74 +528,74 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="2">
-        <v>35714.845000000001</v>
-      </c>
-      <c r="D2">
-        <v>17896.21</v>
+      <c r="B2" s="14"/>
+      <c r="C2" s="10">
+        <v>35714.844999999994</v>
+      </c>
+      <c r="D2" s="13">
+        <v>35807.095000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="2">
+      <c r="B3" s="14"/>
+      <c r="C3" s="11">
         <v>8679.2999999999993</v>
       </c>
-      <c r="D3">
-        <v>11535.5</v>
+      <c r="D3" s="13">
+        <v>7320.4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="2">
+      <c r="B4" s="14"/>
+      <c r="C4" s="11">
         <v>4746.2</v>
       </c>
-      <c r="D4">
-        <v>3529.2000000000003</v>
+      <c r="D4" s="13">
+        <v>2472.6999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="2">
-        <v>0.60270000000000001</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.88919999999999977</v>
+      <c r="B5" s="14"/>
+      <c r="C5" s="12">
+        <v>0.60270000000000046</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.39949999999999974</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="2">
-        <v>1.0084176343828599</v>
-      </c>
-      <c r="D6" s="10">
-        <v>1.0523687869528029</v>
+      <c r="B6" s="14"/>
+      <c r="C6">
+        <v>1.0084176343828561</v>
+      </c>
+      <c r="D6">
+        <v>1.0498713209558093</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="2">
         <v>60</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>60</v>
       </c>
     </row>
@@ -589,11 +620,11 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="8">
-        <v>42489.7</v>
-      </c>
-      <c r="D9" s="8">
-        <v>42177.599999999999</v>
+      <c r="C9" s="9">
+        <v>81453</v>
+      </c>
+      <c r="D9" s="9">
+        <v>48686.8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -603,11 +634,11 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="8">
-        <v>12981.4</v>
-      </c>
-      <c r="D10" s="8">
-        <v>13410.5</v>
+      <c r="C10" s="9">
+        <v>20369.099999999999</v>
+      </c>
+      <c r="D10" s="9">
+        <v>9653.1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -617,11 +648,11 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="8">
-        <v>4944.1000000000004</v>
-      </c>
-      <c r="D11" s="8">
-        <v>4104.6000000000004</v>
+      <c r="C11" s="9">
+        <v>5511</v>
+      </c>
+      <c r="D11" s="9">
+        <v>3195.7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -631,11 +662,11 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="8">
-        <v>3005.1</v>
-      </c>
-      <c r="D12" s="8">
-        <v>2033.4</v>
+      <c r="C12" s="9">
+        <v>2790.7</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1869.4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -645,11 +676,11 @@
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="8">
-        <v>1972.2</v>
-      </c>
-      <c r="D13" s="8">
-        <v>1297</v>
+      <c r="C13" s="9">
+        <v>1933.8</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1460</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -659,11 +690,11 @@
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="8">
-        <v>1521.9</v>
-      </c>
-      <c r="D14" s="8">
-        <v>1041</v>
+      <c r="C14" s="9">
+        <v>1456.8</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1240.0999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -673,11 +704,11 @@
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="8">
-        <v>301.89999999999998</v>
-      </c>
-      <c r="D15" s="8">
-        <v>718.9</v>
+      <c r="C15" s="9">
+        <v>1159.5</v>
+      </c>
+      <c r="D15" s="9">
+        <v>932.4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -687,11 +718,11 @@
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="C16" s="8">
-        <v>1013.6</v>
-      </c>
-      <c r="D16" s="8">
-        <v>616.6</v>
+      <c r="C16" s="9">
+        <v>1015.1</v>
+      </c>
+      <c r="D16" s="9">
+        <v>818.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -701,11 +732,11 @@
       <c r="B17" s="3">
         <v>9</v>
       </c>
-      <c r="C17" s="8">
-        <v>828.6</v>
-      </c>
-      <c r="D17" s="8">
-        <v>513.29999999999995</v>
+      <c r="C17" s="9">
+        <v>882.4</v>
+      </c>
+      <c r="D17" s="9">
+        <v>754</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,11 +746,11 @@
       <c r="B18" s="3">
         <v>10</v>
       </c>
-      <c r="C18" s="8">
-        <v>685.8</v>
-      </c>
-      <c r="D18" s="8">
-        <v>410.2</v>
+      <c r="C18" s="9">
+        <v>788.5</v>
+      </c>
+      <c r="D18" s="9">
+        <v>636.6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -729,11 +760,11 @@
       <c r="B19" s="3">
         <v>11.5</v>
       </c>
-      <c r="C19" s="8">
-        <v>532</v>
-      </c>
-      <c r="D19" s="8">
-        <v>421.1</v>
+      <c r="C19" s="9">
+        <v>801.7</v>
+      </c>
+      <c r="D19" s="9">
+        <v>754.2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,11 +774,11 @@
       <c r="B20" s="3">
         <v>13</v>
       </c>
-      <c r="C20" s="8">
-        <v>503.7</v>
-      </c>
-      <c r="D20" s="8">
-        <v>429.6</v>
+      <c r="C20" s="9">
+        <v>698.5</v>
+      </c>
+      <c r="D20" s="9">
+        <v>692.6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,11 +788,11 @@
       <c r="B21" s="3">
         <v>14.5</v>
       </c>
-      <c r="C21" s="8">
-        <v>576.4</v>
-      </c>
-      <c r="D21" s="8">
-        <v>302.10000000000002</v>
+      <c r="C21" s="9">
+        <v>647.9</v>
+      </c>
+      <c r="D21" s="9">
+        <v>655.7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,11 +802,11 @@
       <c r="B22" s="3">
         <v>16</v>
       </c>
-      <c r="C22" s="8">
-        <v>421.6</v>
-      </c>
-      <c r="D22" s="8">
-        <v>320.5</v>
+      <c r="C22" s="9">
+        <v>629.29999999999995</v>
+      </c>
+      <c r="D22" s="9">
+        <v>551.9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,11 +816,11 @@
       <c r="B23" s="3">
         <v>17.5</v>
       </c>
-      <c r="C23" s="8">
-        <v>403</v>
-      </c>
-      <c r="D23" s="8">
-        <v>291.39999999999998</v>
+      <c r="C23" s="9">
+        <v>622.20000000000005</v>
+      </c>
+      <c r="D23" s="9">
+        <v>593.29999999999995</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -799,11 +830,11 @@
       <c r="B24" s="3">
         <v>19</v>
       </c>
-      <c r="C24" s="8">
-        <v>279.2</v>
-      </c>
-      <c r="D24" s="8">
-        <v>230.4</v>
+      <c r="C24" s="9">
+        <v>507.9</v>
+      </c>
+      <c r="D24" s="9">
+        <v>448.6</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -813,11 +844,11 @@
       <c r="B25" s="3">
         <v>20.5</v>
       </c>
-      <c r="C25" s="8">
-        <v>221.6</v>
-      </c>
-      <c r="D25" s="8">
-        <v>194</v>
+      <c r="C25" s="9">
+        <v>504.2</v>
+      </c>
+      <c r="D25" s="9">
+        <v>480.2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -827,11 +858,11 @@
       <c r="B26" s="3">
         <v>22</v>
       </c>
-      <c r="C26" s="8">
-        <v>245.6</v>
-      </c>
-      <c r="D26" s="8">
-        <v>194.1</v>
+      <c r="C26" s="9">
+        <v>422.8</v>
+      </c>
+      <c r="D26" s="9">
+        <v>437.1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -841,11 +872,11 @@
       <c r="B27" s="3">
         <v>23.5</v>
       </c>
-      <c r="C27" s="8">
-        <v>238.8</v>
-      </c>
-      <c r="D27" s="8">
-        <v>272.10000000000002</v>
+      <c r="C27" s="9">
+        <v>451.9</v>
+      </c>
+      <c r="D27" s="9">
+        <v>429.6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -855,11 +886,11 @@
       <c r="B28" s="3">
         <v>25</v>
       </c>
-      <c r="C28" s="8">
-        <v>225.8</v>
-      </c>
-      <c r="D28" s="8">
-        <v>178.1</v>
+      <c r="C28" s="9">
+        <v>411.3</v>
+      </c>
+      <c r="D28" s="9">
+        <v>299.8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -869,11 +900,11 @@
       <c r="B29" s="3">
         <v>27</v>
       </c>
-      <c r="C29" s="8">
-        <v>250.8</v>
-      </c>
-      <c r="D29" s="8">
-        <v>183.3</v>
+      <c r="C29" s="9">
+        <v>475.7</v>
+      </c>
+      <c r="D29" s="9">
+        <v>471.4</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,11 +914,11 @@
       <c r="B30" s="3">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
-        <v>207</v>
-      </c>
-      <c r="D30" s="8">
-        <v>170.3</v>
+      <c r="C30" s="9">
+        <v>453.3</v>
+      </c>
+      <c r="D30" s="9">
+        <v>375.9</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,11 +928,11 @@
       <c r="B31" s="3">
         <v>31</v>
       </c>
-      <c r="C31" s="8">
-        <v>220.4</v>
-      </c>
-      <c r="D31" s="8">
-        <v>178.6</v>
+      <c r="C31" s="9">
+        <v>467.4</v>
+      </c>
+      <c r="D31" s="9">
+        <v>417.1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,11 +942,11 @@
       <c r="B32" s="3">
         <v>33</v>
       </c>
-      <c r="C32" s="8">
-        <v>236.4</v>
-      </c>
-      <c r="D32" s="8">
-        <v>178.7</v>
+      <c r="C32" s="9">
+        <v>431.2</v>
+      </c>
+      <c r="D32" s="9">
+        <v>398.5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,11 +956,11 @@
       <c r="B33" s="3">
         <v>35</v>
       </c>
-      <c r="C33" s="8">
-        <v>214.7</v>
-      </c>
-      <c r="D33" s="8">
-        <v>163.4</v>
+      <c r="C33" s="9">
+        <v>404.4</v>
+      </c>
+      <c r="D33" s="9">
+        <v>432.2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -939,11 +970,11 @@
       <c r="B34" s="3">
         <v>37</v>
       </c>
-      <c r="C34" s="8">
-        <v>190.1</v>
-      </c>
-      <c r="D34" s="8">
-        <v>143.69999999999999</v>
+      <c r="C34" s="9">
+        <v>432.2</v>
+      </c>
+      <c r="D34" s="9">
+        <v>350.6</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -953,11 +984,11 @@
       <c r="B35" s="3">
         <v>39</v>
       </c>
-      <c r="C35" s="8">
-        <v>205.3</v>
-      </c>
-      <c r="D35" s="8">
-        <v>149.6</v>
+      <c r="C35" s="9">
+        <v>363.8</v>
+      </c>
+      <c r="D35" s="9">
+        <v>355.6</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -967,11 +998,11 @@
       <c r="B36" s="3">
         <v>41</v>
       </c>
-      <c r="C36" s="8">
-        <v>210.8</v>
-      </c>
-      <c r="D36" s="8">
-        <v>150.5</v>
+      <c r="C36" s="9">
+        <v>429.8</v>
+      </c>
+      <c r="D36" s="9">
+        <v>319.5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -981,11 +1012,11 @@
       <c r="B37" s="3">
         <v>43</v>
       </c>
-      <c r="C37" s="8">
-        <v>145.5</v>
-      </c>
-      <c r="D37" s="8">
-        <v>142.5</v>
+      <c r="C37" s="9">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="D37" s="9">
+        <v>259.89999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,11 +1026,11 @@
       <c r="B38" s="4">
         <v>45</v>
       </c>
-      <c r="C38" s="8">
-        <v>151.9</v>
-      </c>
-      <c r="D38" s="8">
-        <v>88.8</v>
+      <c r="C38" s="9">
+        <v>348.1</v>
+      </c>
+      <c r="D38" s="9">
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Almost done creating summary sheet with all data extracted. Found problen in linear regression of pI/II
</commit_message>
<xml_diff>
--- a/CATE Template - Multi Run.xlsx
+++ b/CATE Template - Multi Run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="144525" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Vial #</t>
   </si>
@@ -43,17 +43,20 @@
     <t>Load Time (min)</t>
   </si>
   <si>
-    <t>Fucked</t>
+    <t>Run1</t>
   </si>
   <si>
-    <t>Run1</t>
+    <t>Run2</t>
+  </si>
+  <si>
+    <t>Run5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +81,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -175,11 +182,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -209,10 +217,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -511,23 +525,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -538,8 +555,11 @@
       <c r="D2" s="13">
         <v>35807.095000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="15">
+        <v>7141.4219999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -550,8 +570,11 @@
       <c r="D3" s="13">
         <v>7320.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="16">
+        <v>5170.1000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -562,8 +585,11 @@
       <c r="D4" s="13">
         <v>2472.6999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="16">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
@@ -574,8 +600,11 @@
       <c r="D5" s="13">
         <v>0.39949999999999974</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="17">
+        <v>0.36049999999999915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
@@ -586,8 +615,11 @@
       <c r="D6">
         <v>1.0498713209558093</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="19">
+        <v>1.0245470760959214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>8</v>
       </c>
@@ -598,8 +630,11 @@
       <c r="D7" s="8">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E7" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -626,8 +661,11 @@
       <c r="D9" s="9">
         <v>48686.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="18">
+        <v>52437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -640,8 +678,11 @@
       <c r="D10" s="9">
         <v>9653.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="18">
+        <v>9144.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -654,8 +695,11 @@
       <c r="D11" s="9">
         <v>3195.7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="18">
+        <v>2880.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -668,8 +712,11 @@
       <c r="D12" s="9">
         <v>1869.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="18">
+        <v>1585.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -682,8 +729,11 @@
       <c r="D13" s="9">
         <v>1460</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="18">
+        <v>1156.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -696,8 +746,11 @@
       <c r="D14" s="9">
         <v>1240.0999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="18">
+        <v>923.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -710,8 +763,11 @@
       <c r="D15" s="9">
         <v>932.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="18">
+        <v>788.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -724,8 +780,11 @@
       <c r="D16" s="9">
         <v>818.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="18">
+        <v>720.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
@@ -738,8 +797,11 @@
       <c r="D17" s="9">
         <v>754</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="18">
+        <v>764.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -752,8 +814,11 @@
       <c r="D18" s="9">
         <v>636.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="18">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
@@ -766,8 +831,11 @@
       <c r="D19" s="9">
         <v>754.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="18">
+        <v>644.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -780,8 +848,11 @@
       <c r="D20" s="9">
         <v>692.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="18">
+        <v>738.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
@@ -794,8 +865,11 @@
       <c r="D21" s="9">
         <v>655.7</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="18">
+        <v>549.79999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
@@ -808,8 +882,11 @@
       <c r="D22" s="9">
         <v>551.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="18">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
@@ -822,8 +899,11 @@
       <c r="D23" s="9">
         <v>593.29999999999995</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="18">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16</v>
       </c>
@@ -836,8 +916,11 @@
       <c r="D24" s="9">
         <v>448.6</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="18">
+        <v>496.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17</v>
       </c>
@@ -850,8 +933,11 @@
       <c r="D25" s="9">
         <v>480.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="18">
+        <v>438.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>18</v>
       </c>
@@ -864,8 +950,11 @@
       <c r="D26" s="9">
         <v>437.1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="18">
+        <v>352.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
@@ -878,8 +967,11 @@
       <c r="D27" s="9">
         <v>429.6</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="18">
+        <v>392.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
@@ -892,8 +984,11 @@
       <c r="D28" s="9">
         <v>299.8</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="18">
+        <v>297.89999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>21</v>
       </c>
@@ -906,8 +1001,11 @@
       <c r="D29" s="9">
         <v>471.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="18">
+        <v>472.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>22</v>
       </c>
@@ -920,8 +1018,11 @@
       <c r="D30" s="9">
         <v>375.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="18">
+        <v>382.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>23</v>
       </c>
@@ -934,8 +1035,11 @@
       <c r="D31" s="9">
         <v>417.1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="18">
+        <v>412.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>24</v>
       </c>
@@ -948,8 +1052,11 @@
       <c r="D32" s="9">
         <v>398.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="18">
+        <v>399.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>25</v>
       </c>
@@ -962,8 +1069,11 @@
       <c r="D33" s="9">
         <v>432.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="18">
+        <v>322.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>26</v>
       </c>
@@ -976,8 +1086,11 @@
       <c r="D34" s="9">
         <v>350.6</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="18">
+        <v>375.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>27</v>
       </c>
@@ -990,8 +1103,11 @@
       <c r="D35" s="9">
         <v>355.6</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="18">
+        <v>342.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>28</v>
       </c>
@@ -1004,8 +1120,11 @@
       <c r="D36" s="9">
         <v>319.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="18">
+        <v>387.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>29</v>
       </c>
@@ -1018,8 +1137,11 @@
       <c r="D37" s="9">
         <v>259.89999999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="18">
+        <v>303.89999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>30</v>
       </c>
@@ -1031,6 +1153,9 @@
       </c>
       <c r="D38" s="9">
         <v>325</v>
+      </c>
+      <c r="E38" s="18">
+        <v>324.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>